<commit_message>
Punto de partida: permite evaluar modelo SIN emisiones, pero hasta 2050 con solo importaciones.
</commit_message>
<xml_diff>
--- a/DataBases/Escenarios de Demanda.xlsx
+++ b/DataBases/Escenarios de Demanda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0D6A93-9115-490C-8B53-26F83AABB01D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46EFAFA-CF4F-4B2B-BF99-ED4636787E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Updating (BAU)" sheetId="3" r:id="rId1"/>
@@ -5251,8 +5251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70FAD46C-3E27-4B73-9237-973207CA8095}">
   <dimension ref="C5:DN83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CI19" sqref="CI19"/>
+    <sheetView tabSelected="1" topLeftCell="CF46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="DC61" sqref="DC61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
See ncontro un error en BAU_BLEND_FIX_15
</commit_message>
<xml_diff>
--- a/DataBases/Escenarios de Demanda.xlsx
+++ b/DataBases/Escenarios de Demanda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A8FB2A1-FCB7-4530-9853-A155422EE3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3B95BD-8BE7-4E6E-9AA8-6D8D0E0CBB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Updating (BAU)" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="39">
   <si>
     <t>Año</t>
   </si>
@@ -16474,8 +16474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56E7AC4D-0E7F-418D-918D-47C8BE4942B5}">
   <dimension ref="C5:CU71"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7:Z14"/>
+    <sheetView tabSelected="1" topLeftCell="AT47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BL65" sqref="BL65:BS70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16704,6 +16704,9 @@
         <f>+SUM(W7:Y7)</f>
         <v>31.6646</v>
       </c>
+      <c r="AB7">
+        <v>31.6646</v>
+      </c>
       <c r="AI7" s="1">
         <v>2019</v>
       </c>
@@ -16845,6 +16848,9 @@
         <f>+SUM(W8:Y8)</f>
         <v>30.188499999999998</v>
       </c>
+      <c r="AB8">
+        <v>30.188499999999998</v>
+      </c>
       <c r="AI8" s="1">
         <v>2020</v>
       </c>
@@ -16986,6 +16992,9 @@
         <f t="shared" ref="Z9:Z14" si="11">+SUM(W9:Y9)</f>
         <v>37.356999999999999</v>
       </c>
+      <c r="AB9">
+        <v>37.356999999999999</v>
+      </c>
       <c r="AI9" s="1">
         <v>2025</v>
       </c>
@@ -17125,6 +17134,9 @@
         <f t="shared" si="11"/>
         <v>44.712199999999996</v>
       </c>
+      <c r="AB10">
+        <v>44.712199999999996</v>
+      </c>
       <c r="AI10" s="1">
         <v>2030</v>
       </c>
@@ -17238,6 +17250,9 @@
         <f t="shared" si="11"/>
         <v>53.566800000000001</v>
       </c>
+      <c r="AB11">
+        <v>53.566800000000001</v>
+      </c>
       <c r="AI11" s="1">
         <v>2035</v>
       </c>
@@ -17351,6 +17366,9 @@
         <f t="shared" si="11"/>
         <v>64.202399999999997</v>
       </c>
+      <c r="AB12">
+        <v>64.202399999999997</v>
+      </c>
       <c r="AI12" s="1">
         <v>2040</v>
       </c>
@@ -17464,6 +17482,9 @@
         <f t="shared" si="11"/>
         <v>76.975400000000008</v>
       </c>
+      <c r="AB13">
+        <v>76.975400000000008</v>
+      </c>
       <c r="AI13" s="1">
         <v>2045</v>
       </c>
@@ -17575,6 +17596,9 @@
       </c>
       <c r="Z14">
         <f t="shared" si="11"/>
+        <v>92.31689999999999</v>
+      </c>
+      <c r="AB14">
         <v>92.31689999999999</v>
       </c>
       <c r="AI14" s="1">
@@ -17815,6 +17839,9 @@
         <f>+SUM(W20:X20)</f>
         <v>62.181400000000004</v>
       </c>
+      <c r="AA20">
+        <v>62.181400000000004</v>
+      </c>
       <c r="AI20" s="1">
         <v>2019</v>
       </c>
@@ -17897,6 +17924,9 @@
         <f t="shared" ref="Y21:Y27" si="13">+SUM(W21:X21)</f>
         <v>55.42</v>
       </c>
+      <c r="AA21">
+        <v>55.42</v>
+      </c>
       <c r="AI21" s="1">
         <v>2020</v>
       </c>
@@ -17977,6 +18007,9 @@
         <f t="shared" si="13"/>
         <v>58.573599999999999</v>
       </c>
+      <c r="AA22">
+        <v>58.573599999999999</v>
+      </c>
       <c r="AI22" s="1">
         <v>2025</v>
       </c>
@@ -18031,6 +18064,9 @@
         <f t="shared" si="13"/>
         <v>55.663899999999998</v>
       </c>
+      <c r="AA23">
+        <v>55.663899999999998</v>
+      </c>
       <c r="AI23" s="1">
         <v>2030</v>
       </c>
@@ -18085,6 +18121,9 @@
         <f t="shared" si="13"/>
         <v>54.030799999999999</v>
       </c>
+      <c r="AA24">
+        <v>54.030799999999999</v>
+      </c>
       <c r="AI24" s="1">
         <v>2035</v>
       </c>
@@ -18139,6 +18178,9 @@
         <f t="shared" si="13"/>
         <v>60.668600000000005</v>
       </c>
+      <c r="AA25">
+        <v>60.668600000000005</v>
+      </c>
       <c r="AI25" s="1">
         <v>2040</v>
       </c>
@@ -18193,6 +18235,9 @@
         <f t="shared" si="13"/>
         <v>73.020099999999999</v>
       </c>
+      <c r="AA26">
+        <v>73.020099999999999</v>
+      </c>
       <c r="AI26" s="1">
         <v>2045</v>
       </c>
@@ -18247,6 +18292,9 @@
         <f t="shared" si="13"/>
         <v>88.122200000000007</v>
       </c>
+      <c r="AA27">
+        <v>88.122200000000007</v>
+      </c>
       <c r="AI27" s="1">
         <v>2050</v>
       </c>
@@ -18436,6 +18484,9 @@
         <f>+SUM(W33:X33)</f>
         <v>69.341300000000004</v>
       </c>
+      <c r="AA33">
+        <v>69.341300000000004</v>
+      </c>
       <c r="AI33" s="1">
         <v>2019</v>
       </c>
@@ -18521,6 +18572,9 @@
         <f t="shared" ref="Y34:Y40" si="16">+SUM(W34:X34)</f>
         <v>70.399799999999999</v>
       </c>
+      <c r="AA34">
+        <v>70.399799999999999</v>
+      </c>
       <c r="AI34" s="1">
         <v>2020</v>
       </c>
@@ -18604,6 +18658,9 @@
         <f t="shared" si="16"/>
         <v>72.347100000000012</v>
       </c>
+      <c r="AA35">
+        <v>72.347100000000012</v>
+      </c>
       <c r="AI35" s="1">
         <v>2025</v>
       </c>
@@ -18661,6 +18718,9 @@
         <f t="shared" si="16"/>
         <v>60.032299999999999</v>
       </c>
+      <c r="AA36">
+        <v>60.032299999999999</v>
+      </c>
       <c r="AI36" s="1">
         <v>2030</v>
       </c>
@@ -18718,6 +18778,9 @@
         <f t="shared" si="16"/>
         <v>40.972300000000004</v>
       </c>
+      <c r="AA37">
+        <v>40.972300000000004</v>
+      </c>
       <c r="AI37" s="1">
         <v>2035</v>
       </c>
@@ -18775,6 +18838,9 @@
         <f t="shared" si="16"/>
         <v>26.482499999999998</v>
       </c>
+      <c r="AA38">
+        <v>26.482499999999998</v>
+      </c>
       <c r="AI38" s="1">
         <v>2040</v>
       </c>
@@ -18832,6 +18898,9 @@
         <f t="shared" si="16"/>
         <v>15.279199999999999</v>
       </c>
+      <c r="AA39">
+        <v>15.279199999999999</v>
+      </c>
       <c r="AI39" s="1">
         <v>2045</v>
       </c>
@@ -18889,6 +18958,9 @@
         <f t="shared" si="16"/>
         <v>7.4989999999999997</v>
       </c>
+      <c r="AA40">
+        <v>7.4989999999999997</v>
+      </c>
       <c r="AI40" s="1">
         <v>2050</v>
       </c>
@@ -19219,6 +19291,9 @@
         <f t="shared" ref="AE48:AE55" si="19">+SUM(W48:AD48)</f>
         <v>105.9659</v>
       </c>
+      <c r="AF48">
+        <v>105.9659</v>
+      </c>
       <c r="AI48" s="1">
         <v>2019</v>
       </c>
@@ -19396,6 +19471,9 @@
         <f t="shared" si="19"/>
         <v>98.641600000000011</v>
       </c>
+      <c r="AF49">
+        <v>98.641600000000011</v>
+      </c>
       <c r="AI49" s="1">
         <v>2020</v>
       </c>
@@ -19573,6 +19651,9 @@
         <f t="shared" si="19"/>
         <v>109.53559999999999</v>
       </c>
+      <c r="AF50">
+        <v>109.53559999999999</v>
+      </c>
       <c r="AI50" s="1">
         <v>2025</v>
       </c>
@@ -19750,6 +19831,9 @@
         <f t="shared" si="19"/>
         <v>115.2475</v>
       </c>
+      <c r="AF51">
+        <v>115.2475</v>
+      </c>
       <c r="AI51" s="1">
         <v>2030</v>
       </c>
@@ -19927,6 +20011,9 @@
         <f t="shared" si="19"/>
         <v>122.26180000000001</v>
       </c>
+      <c r="AF52">
+        <v>122.26180000000001</v>
+      </c>
       <c r="AI52" s="1">
         <v>2035</v>
       </c>
@@ -20104,6 +20191,9 @@
         <f t="shared" si="19"/>
         <v>136.90830000000003</v>
       </c>
+      <c r="AF53">
+        <v>136.90830000000003</v>
+      </c>
       <c r="AI53" s="1">
         <v>2040</v>
       </c>
@@ -20281,6 +20371,9 @@
         <f t="shared" si="19"/>
         <v>158.66909999999996</v>
       </c>
+      <c r="AF54">
+        <v>158.66909999999996</v>
+      </c>
       <c r="AI54" s="1">
         <v>2045</v>
       </c>
@@ -20456,6 +20549,9 @@
       </c>
       <c r="AE55">
         <f t="shared" si="19"/>
+        <v>185.6712</v>
+      </c>
+      <c r="AF55">
         <v>185.6712</v>
       </c>
       <c r="AI55" s="1">
@@ -20840,6 +20936,9 @@
         <f t="shared" ref="AE64:AE71" si="23">+SUM(W64:AD64)</f>
         <v>574.73889999999994</v>
       </c>
+      <c r="AF64">
+        <v>574.73889999999994</v>
+      </c>
       <c r="AI64" s="1">
         <v>2019</v>
       </c>
@@ -20999,6 +21098,9 @@
         <f t="shared" si="23"/>
         <v>577.1468000000001</v>
       </c>
+      <c r="AF65">
+        <v>577.1468000000001</v>
+      </c>
       <c r="AI65" s="1">
         <v>2020</v>
       </c>
@@ -21158,6 +21260,9 @@
         <f t="shared" si="23"/>
         <v>648.25800000000004</v>
       </c>
+      <c r="AF66">
+        <v>648.25800000000004</v>
+      </c>
       <c r="AI66" s="1">
         <v>2025</v>
       </c>
@@ -21317,6 +21422,9 @@
         <f t="shared" si="23"/>
         <v>691.68829999999991</v>
       </c>
+      <c r="AF67">
+        <v>691.68829999999991</v>
+      </c>
       <c r="AI67" s="1">
         <v>2030</v>
       </c>
@@ -21476,6 +21584,9 @@
         <f t="shared" si="23"/>
         <v>700.2876</v>
       </c>
+      <c r="AF68">
+        <v>700.2876</v>
+      </c>
       <c r="AI68" s="1">
         <v>2035</v>
       </c>
@@ -21635,6 +21746,9 @@
         <f t="shared" si="23"/>
         <v>696.71199999999999</v>
       </c>
+      <c r="AF69">
+        <v>696.71199999999999</v>
+      </c>
       <c r="AI69" s="1">
         <v>2040</v>
       </c>
@@ -21794,6 +21908,9 @@
         <f t="shared" si="23"/>
         <v>689.51819999999998</v>
       </c>
+      <c r="AF70">
+        <v>689.51819999999998</v>
+      </c>
       <c r="AI70" s="1">
         <v>2045</v>
       </c>
@@ -21951,6 +22068,9 @@
       </c>
       <c r="AE71">
         <f t="shared" si="23"/>
+        <v>693.02160000000003</v>
+      </c>
+      <c r="AF71">
         <v>693.02160000000003</v>
       </c>
       <c r="AI71" s="1">
@@ -22054,10 +22174,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36743DA1-B432-473B-8C13-5675963D3C1A}">
-  <dimension ref="C5:BQ71"/>
+  <dimension ref="C5:CV133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AG64" sqref="AG64:AG71"/>
+    <sheetView topLeftCell="AH45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AW50" sqref="AW50:BD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22068,11 +22188,12 @@
     <col min="25" max="25" width="12" customWidth="1"/>
     <col min="34" max="34" width="9.140625" style="21"/>
     <col min="37" max="37" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="48" max="56" width="0" hidden="1" customWidth="1"/>
-    <col min="57" max="57" width="9.140625" style="5"/>
+    <col min="48" max="48" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="79" max="87" width="0" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -22092,7 +22213,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="3:69" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:100" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
@@ -22135,38 +22256,66 @@
       <c r="AM6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BG6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BH6" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="BI6" s="12" t="s">
+      <c r="AQ6" t="str" cm="1">
+        <f t="array" ref="AQ6:AY9">+TRANSPOSE(AJ6:AM14)</f>
+        <v>Año</v>
+      </c>
+      <c r="AR6">
+        <v>2019</v>
+      </c>
+      <c r="AS6">
+        <v>2020</v>
+      </c>
+      <c r="AT6">
+        <v>2025</v>
+      </c>
+      <c r="AU6">
+        <v>2030</v>
+      </c>
+      <c r="AV6">
+        <v>2035</v>
+      </c>
+      <c r="AW6">
+        <v>2040</v>
+      </c>
+      <c r="AX6">
+        <v>2045</v>
+      </c>
+      <c r="AY6">
+        <v>2050</v>
+      </c>
+      <c r="CL6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM6" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="CN6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="BJ6" s="12" t="s">
+      <c r="CO6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="BK6" s="12" t="s">
+      <c r="CP6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="BL6" s="12" t="s">
+      <c r="CQ6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="BM6" s="12" t="s">
+      <c r="CR6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="BN6" s="12" t="s">
+      <c r="CS6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="BO6" s="10" t="s">
+      <c r="CT6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="BP6" s="12" t="s">
+      <c r="CU6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1">
         <v>2019</v>
       </c>
@@ -22226,51 +22375,78 @@
         <f>+SUM(AK7:AM7)</f>
         <v>1</v>
       </c>
-      <c r="BG7" s="11">
+      <c r="AQ7" t="str">
+        <v>Diésel</v>
+      </c>
+      <c r="AR7" s="35">
+        <v>0.70492284759636947</v>
+      </c>
+      <c r="AS7" s="35">
+        <v>0.71027709227023539</v>
+      </c>
+      <c r="AT7" s="35">
+        <v>0.71018283052707665</v>
+      </c>
+      <c r="AU7" s="35">
+        <v>0.71320579170785603</v>
+      </c>
+      <c r="AV7" s="35">
+        <v>0.71486629778146171</v>
+      </c>
+      <c r="AW7" s="35">
+        <v>0.71503401741990957</v>
+      </c>
+      <c r="AX7" s="35">
+        <v>0.71399693928190033</v>
+      </c>
+      <c r="AY7" s="35">
+        <v>0.71196823116894092</v>
+      </c>
+      <c r="CL7" s="11">
         <v>2019</v>
       </c>
-      <c r="BH7" s="13">
+      <c r="CM7" s="13">
         <f>+W7+W48+W64</f>
         <v>269.4325</v>
       </c>
-      <c r="BI7" s="14">
+      <c r="CN7" s="14">
         <f>+X7+X48+X64</f>
         <v>249.2398</v>
       </c>
-      <c r="BJ7" s="14">
-        <f t="shared" ref="BJ7:BJ14" si="0">+Y7+W20+W33+Y48+Y64</f>
+      <c r="CO7" s="14">
+        <f t="shared" ref="CO7:CO14" si="0">+Y7+W20+W33+Y48+Y64</f>
         <v>238.81580000000002</v>
       </c>
-      <c r="BK7" s="14">
-        <f t="shared" ref="BK7:BK14" si="1">+Z48+Z64</f>
+      <c r="CP7" s="14">
+        <f t="shared" ref="CP7:CP14" si="1">+Z48+Z64</f>
         <v>59.134499999999996</v>
       </c>
-      <c r="BL7" s="14">
-        <f t="shared" ref="BL7:BL14" si="2">+X20+X33+AA48+AA64</f>
+      <c r="CQ7" s="14">
+        <f t="shared" ref="CQ7:CQ14" si="2">+X20+X33+AA48+AA64</f>
         <v>25.486199999999997</v>
       </c>
-      <c r="BM7" s="14">
+      <c r="CR7" s="14">
         <f>+AB48+AB64</f>
         <v>1.1855</v>
       </c>
-      <c r="BN7" s="14">
+      <c r="CS7" s="14">
         <f>+AC48</f>
         <v>7.3300000000000004E-2</v>
       </c>
-      <c r="BO7" s="14">
+      <c r="CT7" s="14">
         <f>+AC64</f>
         <v>0.52449999999999997</v>
       </c>
-      <c r="BP7" s="15">
-        <f t="shared" ref="BP7:BP14" si="3">+AD48+AD64</f>
-        <v>0</v>
-      </c>
-      <c r="BQ7" s="21">
-        <f>+SUM(BH7:BP7)</f>
+      <c r="CU7" s="15">
+        <f t="shared" ref="CU7:CU14" si="3">+AD48+AD64</f>
+        <v>0</v>
+      </c>
+      <c r="CV7" s="21">
+        <f>+SUM(CM7:CU7)</f>
         <v>843.89210000000003</v>
       </c>
     </row>
-    <row r="8" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" s="1">
         <v>2020</v>
       </c>
@@ -22316,62 +22492,89 @@
         <v>0.71027709227023539</v>
       </c>
       <c r="AL8" s="23">
-        <f>+X8/$Z8</f>
+        <f t="shared" ref="AL8:AM14" si="5">+X8/$Z8</f>
         <v>6.929791145634928E-3</v>
       </c>
       <c r="AM8" s="23">
-        <f>+Y8/$Z8</f>
+        <f t="shared" si="5"/>
         <v>0.28279311658412976</v>
       </c>
       <c r="AN8">
         <f>+SUM(AK8:AM8)</f>
         <v>1</v>
       </c>
-      <c r="BG8" s="11">
+      <c r="AQ8" t="str">
+        <v>Gasolina</v>
+      </c>
+      <c r="AR8" s="35">
+        <v>6.6920156894449958E-3</v>
+      </c>
+      <c r="AS8" s="35">
+        <v>6.929791145634928E-3</v>
+      </c>
+      <c r="AT8" s="35">
+        <v>6.77249243782959E-3</v>
+      </c>
+      <c r="AU8" s="35">
+        <v>6.6178805784550977E-3</v>
+      </c>
+      <c r="AV8" s="35">
+        <v>6.5021617867783779E-3</v>
+      </c>
+      <c r="AW8" s="35">
+        <v>6.4218783098451155E-3</v>
+      </c>
+      <c r="AX8" s="35">
+        <v>6.3682683038996874E-3</v>
+      </c>
+      <c r="AY8" s="35">
+        <v>6.3368678974272319E-3</v>
+      </c>
+      <c r="CL8" s="11">
         <v>2020</v>
       </c>
-      <c r="BH8" s="16">
+      <c r="CM8" s="16">
         <f>+W8+W49+W65</f>
         <v>276.96129999999999</v>
       </c>
-      <c r="BI8">
+      <c r="CN8">
         <f>+X8+X49+X65</f>
         <v>256.4101</v>
       </c>
-      <c r="BJ8">
+      <c r="CO8">
         <f t="shared" si="0"/>
         <v>224.12989999999999</v>
       </c>
-      <c r="BK8">
+      <c r="CP8">
         <f t="shared" si="1"/>
         <v>47.282299999999999</v>
       </c>
-      <c r="BL8">
+      <c r="CQ8">
         <f t="shared" si="2"/>
         <v>25.2714</v>
       </c>
-      <c r="BM8">
-        <f t="shared" ref="BM8:BM14" si="5">+AB49+AB65</f>
+      <c r="CR8">
+        <f t="shared" ref="CR8:CR14" si="6">+AB49+AB65</f>
         <v>1.2454000000000001</v>
       </c>
-      <c r="BN8">
-        <f t="shared" ref="BN8:BN14" si="6">+AC49</f>
+      <c r="CS8">
+        <f t="shared" ref="CS8:CS14" si="7">+AC49</f>
         <v>6.9099999999999995E-2</v>
       </c>
-      <c r="BO8">
-        <f t="shared" ref="BO8:BO14" si="7">+AC65</f>
-        <v>0</v>
-      </c>
-      <c r="BP8" s="17">
+      <c r="CT8">
+        <f t="shared" ref="CT8:CT14" si="8">+AC65</f>
+        <v>0</v>
+      </c>
+      <c r="CU8" s="17">
         <f t="shared" si="3"/>
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="BQ8" s="21">
-        <f t="shared" ref="BQ8:BQ14" si="8">+SUM(BH8:BP8)</f>
+      <c r="CV8" s="21">
+        <f t="shared" ref="CV8:CV14" si="9">+SUM(CM8:CU8)</f>
         <v>831.3759</v>
       </c>
     </row>
-    <row r="9" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="1">
         <v>2025</v>
       </c>
@@ -22403,7 +22606,7 @@
         <v>10.573700000000001</v>
       </c>
       <c r="Z9">
-        <f t="shared" ref="Z9:Z14" si="9">+SUM(W9:Y9)</f>
+        <f t="shared" ref="Z9:Z14" si="10">+SUM(W9:Y9)</f>
         <v>37.356999999999999</v>
       </c>
       <c r="AB9">
@@ -22417,62 +22620,89 @@
         <v>0.71018283052707665</v>
       </c>
       <c r="AL9" s="23">
-        <f>+X9/$Z9</f>
+        <f t="shared" si="5"/>
         <v>6.77249243782959E-3</v>
       </c>
       <c r="AM9" s="23">
-        <f>+Y9/$Z9</f>
+        <f t="shared" si="5"/>
         <v>0.28304467703509384</v>
       </c>
       <c r="AN9">
-        <f t="shared" ref="AN9:AN14" si="10">+SUM(AK9:AM9)</f>
-        <v>1</v>
-      </c>
-      <c r="BG9" s="11">
+        <f t="shared" ref="AN9:AN14" si="11">+SUM(AK9:AM9)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ9" t="str">
+        <v>Gas Natural</v>
+      </c>
+      <c r="AR9" s="35">
+        <v>0.28838513671418559</v>
+      </c>
+      <c r="AS9" s="35">
+        <v>0.28279311658412976</v>
+      </c>
+      <c r="AT9" s="35">
+        <v>0.28304467703509384</v>
+      </c>
+      <c r="AU9" s="35">
+        <v>0.28017632771368889</v>
+      </c>
+      <c r="AV9" s="35">
+        <v>0.27863154043175997</v>
+      </c>
+      <c r="AW9" s="35">
+        <v>0.27854410427024534</v>
+      </c>
+      <c r="AX9" s="35">
+        <v>0.27963479241419981</v>
+      </c>
+      <c r="AY9" s="35">
+        <v>0.28169490093363186</v>
+      </c>
+      <c r="CL9" s="11">
         <v>2025</v>
       </c>
-      <c r="BH9" s="16">
+      <c r="CM9" s="16">
         <f>+W9+W50+W66</f>
         <v>301.00240000000002</v>
       </c>
-      <c r="BI9">
+      <c r="CN9">
         <f>+X9+X50+X66</f>
         <v>258.53140000000002</v>
       </c>
-      <c r="BJ9">
+      <c r="CO9">
         <f t="shared" si="0"/>
         <v>234.21699999999998</v>
       </c>
-      <c r="BK9">
+      <c r="CP9">
         <f t="shared" si="1"/>
         <v>57.954099999999997</v>
       </c>
-      <c r="BL9">
+      <c r="CQ9">
         <f t="shared" si="2"/>
         <v>21.922500000000003</v>
       </c>
-      <c r="BM9">
-        <f t="shared" si="5"/>
+      <c r="CR9">
+        <f t="shared" si="6"/>
         <v>1.3845000000000001</v>
       </c>
-      <c r="BN9">
-        <f t="shared" si="6"/>
+      <c r="CS9">
+        <f t="shared" si="7"/>
         <v>3.7600000000000001E-2</v>
       </c>
-      <c r="BO9">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="BP9" s="17">
+      <c r="CT9">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU9" s="17">
         <f t="shared" si="3"/>
         <v>0.20419999999999999</v>
       </c>
-      <c r="BQ9" s="21">
-        <f t="shared" si="8"/>
+      <c r="CV9" s="21">
+        <f t="shared" si="9"/>
         <v>875.25370000000009</v>
       </c>
     </row>
-    <row r="10" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>2030</v>
       </c>
@@ -22504,7 +22734,7 @@
         <v>12.5273</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>44.712199999999996</v>
       </c>
       <c r="AB10">
@@ -22518,62 +22748,62 @@
         <v>0.71320579170785603</v>
       </c>
       <c r="AL10" s="23">
-        <f>+X10/$Z10</f>
+        <f t="shared" si="5"/>
         <v>6.6178805784550977E-3</v>
       </c>
       <c r="AM10" s="23">
-        <f>+Y10/$Z10</f>
+        <f t="shared" si="5"/>
         <v>0.28017632771368889</v>
       </c>
       <c r="AN10">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="BG10" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="CL10" s="11">
         <v>2030</v>
       </c>
-      <c r="BH10" s="16">
+      <c r="CM10" s="16">
         <f>+W10+W51+W67</f>
         <v>310.70049999999998</v>
       </c>
-      <c r="BI10">
+      <c r="CN10">
         <f>+X10+X51+X67</f>
         <v>236.68710000000002</v>
       </c>
-      <c r="BJ10">
+      <c r="CO10">
         <f t="shared" si="0"/>
         <v>206.82849999999999</v>
       </c>
-      <c r="BK10">
+      <c r="CP10">
         <f t="shared" si="1"/>
         <v>69.258200000000002</v>
       </c>
-      <c r="BL10">
+      <c r="CQ10">
         <f t="shared" si="2"/>
         <v>14.055299999999999</v>
       </c>
-      <c r="BM10">
-        <f t="shared" si="5"/>
+      <c r="CR10">
+        <f t="shared" si="6"/>
         <v>1.5010000000000001</v>
       </c>
-      <c r="BN10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BO10">
+      <c r="CS10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BP10" s="17">
+      <c r="CT10">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU10" s="17">
         <f t="shared" si="3"/>
         <v>22.426299999999998</v>
       </c>
-      <c r="BQ10" s="21">
-        <f t="shared" si="8"/>
+      <c r="CV10" s="21">
+        <f t="shared" si="9"/>
         <v>861.45689999999991</v>
       </c>
     </row>
-    <row r="11" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="1">
         <v>2035</v>
       </c>
@@ -22605,7 +22835,7 @@
         <v>14.9254</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>53.566800000000001</v>
       </c>
       <c r="AB11">
@@ -22619,62 +22849,62 @@
         <v>0.71486629778146171</v>
       </c>
       <c r="AL11" s="23">
-        <f>+X11/$Z11</f>
+        <f t="shared" si="5"/>
         <v>6.5021617867783779E-3</v>
       </c>
       <c r="AM11" s="23">
-        <f>+Y11/$Z11</f>
+        <f t="shared" si="5"/>
         <v>0.27863154043175997</v>
       </c>
       <c r="AN11">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="BG11" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="CL11" s="11">
         <v>2035</v>
       </c>
-      <c r="BH11" s="16">
+      <c r="CM11" s="16">
         <f>+W11+W52+W68</f>
         <v>309.00689999999997</v>
       </c>
-      <c r="BI11">
+      <c r="CN11">
         <f>+X11+X52+X68</f>
         <v>200.9239</v>
       </c>
-      <c r="BJ11">
+      <c r="CO11">
         <f t="shared" si="0"/>
         <v>207.6635</v>
       </c>
-      <c r="BK11">
+      <c r="CP11">
         <f t="shared" si="1"/>
         <v>82.876599999999996</v>
       </c>
-      <c r="BL11">
+      <c r="CQ11">
         <f t="shared" si="2"/>
         <v>12.142300000000001</v>
       </c>
-      <c r="BM11">
-        <f t="shared" si="5"/>
+      <c r="CR11">
+        <f t="shared" si="6"/>
         <v>1.7801999999999998</v>
       </c>
-      <c r="BN11">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BO11">
+      <c r="CS11">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BP11" s="17">
+      <c r="CT11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU11" s="17">
         <f t="shared" si="3"/>
         <v>43.486399999999996</v>
       </c>
-      <c r="BQ11" s="21">
-        <f t="shared" si="8"/>
+      <c r="CV11" s="21">
+        <f t="shared" si="9"/>
         <v>857.87980000000005</v>
       </c>
     </row>
-    <row r="12" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1">
         <v>2040</v>
       </c>
@@ -22706,7 +22936,7 @@
         <v>17.883199999999999</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>64.202399999999997</v>
       </c>
       <c r="AB12">
@@ -22720,62 +22950,62 @@
         <v>0.71503401741990957</v>
       </c>
       <c r="AL12" s="23">
-        <f>+X12/$Z12</f>
+        <f t="shared" si="5"/>
         <v>6.4218783098451155E-3</v>
       </c>
       <c r="AM12" s="23">
-        <f>+Y12/$Z12</f>
+        <f t="shared" si="5"/>
         <v>0.27854410427024534</v>
       </c>
       <c r="AN12">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="BG12" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="CL12" s="11">
         <v>2040</v>
       </c>
-      <c r="BH12" s="16">
+      <c r="CM12" s="16">
         <f>+W12+W53+W69</f>
         <v>295.27800000000002</v>
       </c>
-      <c r="BI12">
+      <c r="CN12">
         <f>+X12+X53+X69</f>
         <v>159.23560000000001</v>
       </c>
-      <c r="BJ12">
+      <c r="CO12">
         <f t="shared" si="0"/>
         <v>235.07699999999997</v>
       </c>
-      <c r="BK12">
+      <c r="CP12">
         <f t="shared" si="1"/>
         <v>99.271299999999997</v>
       </c>
-      <c r="BL12">
+      <c r="CQ12">
         <f t="shared" si="2"/>
         <v>12.507</v>
       </c>
-      <c r="BM12">
-        <f t="shared" si="5"/>
+      <c r="CR12">
+        <f t="shared" si="6"/>
         <v>2.1221999999999999</v>
       </c>
-      <c r="BN12">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BO12">
+      <c r="CS12">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BP12" s="17">
+      <c r="CT12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU12" s="17">
         <f t="shared" si="3"/>
         <v>77.346199999999996</v>
       </c>
-      <c r="BQ12" s="21">
-        <f t="shared" si="8"/>
+      <c r="CV12" s="21">
+        <f t="shared" si="9"/>
         <v>880.83729999999991</v>
       </c>
     </row>
-    <row r="13" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="1">
         <v>2045</v>
       </c>
@@ -22807,7 +23037,7 @@
         <v>21.524999999999999</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>76.975400000000008</v>
       </c>
       <c r="AB13">
@@ -22821,62 +23051,62 @@
         <v>0.71399693928190033</v>
       </c>
       <c r="AL13" s="23">
-        <f>+X13/$Z13</f>
+        <f t="shared" si="5"/>
         <v>6.3682683038996874E-3</v>
       </c>
       <c r="AM13" s="23">
-        <f>+Y13/$Z13</f>
+        <f t="shared" si="5"/>
         <v>0.27963479241419981</v>
       </c>
       <c r="AN13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.99999999999999978</v>
       </c>
-      <c r="BG13" s="11">
+      <c r="CL13" s="11">
         <v>2045</v>
       </c>
-      <c r="BH13" s="16">
+      <c r="CM13" s="16">
         <f>+W13+W54+W70</f>
         <v>268.9359</v>
       </c>
-      <c r="BI13">
+      <c r="CN13">
         <f>+X13+X54+X70</f>
         <v>119.3944</v>
       </c>
-      <c r="BJ13">
+      <c r="CO13">
         <f t="shared" si="0"/>
         <v>291.46449999999999</v>
       </c>
-      <c r="BK13">
+      <c r="CP13">
         <f t="shared" si="1"/>
         <v>119.0154</v>
       </c>
-      <c r="BL13">
+      <c r="CQ13">
         <f t="shared" si="2"/>
         <v>13.044</v>
       </c>
-      <c r="BM13">
-        <f t="shared" si="5"/>
+      <c r="CR13">
+        <f t="shared" si="6"/>
         <v>2.5340000000000003</v>
       </c>
-      <c r="BN13">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BO13">
+      <c r="CS13">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BP13" s="17">
+      <c r="CT13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU13" s="17">
         <f t="shared" si="3"/>
         <v>102.64410000000001</v>
       </c>
-      <c r="BQ13" s="21">
-        <f t="shared" si="8"/>
+      <c r="CV13" s="21">
+        <f t="shared" si="9"/>
         <v>917.03229999999996</v>
       </c>
     </row>
-    <row r="14" spans="3:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:100" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="1">
         <v>2050</v>
       </c>
@@ -22908,7 +23138,7 @@
         <v>26.005199999999999</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>92.31689999999999</v>
       </c>
       <c r="AB14">
@@ -22922,67 +23152,67 @@
         <v>0.71196823116894092</v>
       </c>
       <c r="AL14" s="23">
-        <f>+X14/$Z14</f>
+        <f t="shared" si="5"/>
         <v>6.3368678974272319E-3</v>
       </c>
       <c r="AM14" s="23">
-        <f>+Y14/$Z14</f>
+        <f t="shared" si="5"/>
         <v>0.28169490093363186</v>
       </c>
       <c r="AN14">
-        <f t="shared" si="10"/>
-        <v>1</v>
-      </c>
-      <c r="BG14" s="11">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="CL14" s="11">
         <v>2050</v>
       </c>
-      <c r="BH14" s="18">
+      <c r="CM14" s="18">
         <f>+W14+W55+W71</f>
         <v>243.03859999999997</v>
       </c>
-      <c r="BI14" s="19">
+      <c r="CN14" s="19">
         <f>+X14+X55+X71</f>
         <v>85.105699999999999</v>
       </c>
-      <c r="BJ14" s="19">
+      <c r="CO14" s="19">
         <f t="shared" si="0"/>
         <v>356.22730000000001</v>
       </c>
-      <c r="BK14" s="19">
+      <c r="CP14" s="19">
         <f t="shared" si="1"/>
         <v>142.80629999999999</v>
       </c>
-      <c r="BL14" s="19">
+      <c r="CQ14" s="19">
         <f t="shared" si="2"/>
         <v>13.2254</v>
       </c>
-      <c r="BM14" s="19">
-        <f t="shared" si="5"/>
+      <c r="CR14" s="19">
+        <f t="shared" si="6"/>
         <v>3.0295000000000001</v>
       </c>
-      <c r="BN14" s="19">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="BO14" s="19">
+      <c r="CS14" s="19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="BP14" s="20">
+      <c r="CT14" s="19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="CU14" s="20">
         <f t="shared" si="3"/>
         <v>129.72829999999999</v>
       </c>
-      <c r="BQ14" s="21">
-        <f t="shared" si="8"/>
+      <c r="CV14" s="21">
+        <f t="shared" si="9"/>
         <v>973.16109999999992</v>
       </c>
     </row>
-    <row r="15" spans="3:69" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:100" x14ac:dyDescent="0.25">
       <c r="W15" s="22"/>
       <c r="X15" s="22"/>
       <c r="Y15" s="22"/>
     </row>
-    <row r="18" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>8</v>
       </c>
@@ -23002,7 +23232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="3:39" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:51" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C19" s="1" t="s">
         <v>0</v>
       </c>
@@ -23033,8 +23263,36 @@
       <c r="AL19" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="AQ19" t="str" cm="1">
+        <f t="array" ref="AQ19:AY21">+TRANSPOSE(AJ19:AL27)</f>
+        <v>Año</v>
+      </c>
+      <c r="AR19">
+        <v>2019</v>
+      </c>
+      <c r="AS19">
+        <v>2020</v>
+      </c>
+      <c r="AT19">
+        <v>2025</v>
+      </c>
+      <c r="AU19">
+        <v>2030</v>
+      </c>
+      <c r="AV19">
+        <v>2035</v>
+      </c>
+      <c r="AW19">
+        <v>2040</v>
+      </c>
+      <c r="AX19">
+        <v>2045</v>
+      </c>
+      <c r="AY19">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="20" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="1">
         <v>2019</v>
       </c>
@@ -23059,7 +23317,7 @@
         <v>3.1621000000000001</v>
       </c>
       <c r="Y20">
-        <f>+SUM(W20:X20)</f>
+        <f t="shared" ref="Y20:Y27" si="12">+SUM(W20:X20)</f>
         <v>62.181400000000004</v>
       </c>
       <c r="AB20">
@@ -23069,19 +23327,46 @@
         <v>2019</v>
       </c>
       <c r="AK20" s="24">
-        <f>+W20/$Y20</f>
+        <f t="shared" ref="AK20:AL27" si="13">+W20/$Y20</f>
         <v>0.94914717262718429</v>
       </c>
       <c r="AL20" s="24">
-        <f>+X20/$Y20</f>
+        <f t="shared" si="13"/>
         <v>5.0852827372815664E-2</v>
       </c>
       <c r="AM20">
         <f>+SUM(AK20:AL20)</f>
         <v>1</v>
       </c>
+      <c r="AQ20" t="str">
+        <v>Gas Natural</v>
+      </c>
+      <c r="AR20" s="35">
+        <v>0.94914717262718429</v>
+      </c>
+      <c r="AS20" s="35">
+        <v>0.94891867558097909</v>
+      </c>
+      <c r="AT20" s="35">
+        <v>0.93974905303030309</v>
+      </c>
+      <c r="AU20" s="35">
+        <v>0.96760169800742202</v>
+      </c>
+      <c r="AV20" s="35">
+        <v>0.99894955266461494</v>
+      </c>
+      <c r="AW20" s="35">
+        <v>1</v>
+      </c>
+      <c r="AX20" s="35">
+        <v>1</v>
+      </c>
+      <c r="AY20" s="35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1">
         <v>2020</v>
       </c>
@@ -23104,7 +23389,7 @@
         <v>2.8254000000000001</v>
       </c>
       <c r="Y21">
-        <f>+SUM(W21:X21)</f>
+        <f t="shared" si="12"/>
         <v>55.311800000000005</v>
       </c>
       <c r="AB21">
@@ -23114,19 +23399,46 @@
         <v>2020</v>
       </c>
       <c r="AK21" s="24">
-        <f>+W21/$Y21</f>
+        <f t="shared" si="13"/>
         <v>0.94891867558097909</v>
       </c>
       <c r="AL21" s="24">
-        <f>+X21/$Y21</f>
+        <f t="shared" si="13"/>
         <v>5.1081324419020892E-2</v>
       </c>
       <c r="AM21">
-        <f t="shared" ref="AM21:AM27" si="11">+SUM(AK21:AL21)</f>
-        <v>1</v>
+        <f t="shared" ref="AM21:AM27" si="14">+SUM(AK21:AL21)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ21" t="str">
+        <v>GLP</v>
+      </c>
+      <c r="AR21" s="35">
+        <v>5.0852827372815664E-2</v>
+      </c>
+      <c r="AS21" s="35">
+        <v>5.1081324419020892E-2</v>
+      </c>
+      <c r="AT21" s="35">
+        <v>6.0250946969696968E-2</v>
+      </c>
+      <c r="AU21" s="35">
+        <v>3.2398301992577885E-2</v>
+      </c>
+      <c r="AV21" s="35">
+        <v>1.050447335385154E-3</v>
+      </c>
+      <c r="AW21" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX21" s="35">
+        <v>0</v>
+      </c>
+      <c r="AY21" s="35">
+        <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1">
         <v>2025</v>
       </c>
@@ -23149,7 +23461,7 @@
         <v>3.2576000000000001</v>
       </c>
       <c r="Y22">
-        <f>+SUM(W22:X22)</f>
+        <f t="shared" si="12"/>
         <v>54.0672</v>
       </c>
       <c r="AB22">
@@ -23159,19 +23471,19 @@
         <v>2025</v>
       </c>
       <c r="AK22" s="24">
-        <f>+W22/$Y22</f>
+        <f t="shared" si="13"/>
         <v>0.93974905303030309</v>
       </c>
       <c r="AL22" s="24">
-        <f>+X22/$Y22</f>
+        <f t="shared" si="13"/>
         <v>6.0250946969696968E-2</v>
       </c>
       <c r="AM22">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1">
         <v>2030</v>
       </c>
@@ -23194,7 +23506,7 @@
         <v>1.4561999999999999</v>
       </c>
       <c r="Y23">
-        <f>+SUM(W23:X23)</f>
+        <f t="shared" si="12"/>
         <v>44.946800000000003</v>
       </c>
       <c r="AB23">
@@ -23204,19 +23516,19 @@
         <v>2030</v>
       </c>
       <c r="AK23" s="24">
-        <f>+W23/$Y23</f>
+        <f t="shared" si="13"/>
         <v>0.96760169800742202</v>
       </c>
       <c r="AL23" s="24">
-        <f>+X23/$Y23</f>
+        <f t="shared" si="13"/>
         <v>3.2398301992577885E-2</v>
       </c>
       <c r="AM23">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.99999999999999989</v>
       </c>
     </row>
-    <row r="24" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="1">
         <v>2035</v>
       </c>
@@ -23239,7 +23551,7 @@
         <v>5.28E-2</v>
       </c>
       <c r="Y24">
-        <f>+SUM(W24:X24)</f>
+        <f t="shared" si="12"/>
         <v>50.264299999999999</v>
       </c>
       <c r="AB24">
@@ -23249,19 +23561,19 @@
         <v>2035</v>
       </c>
       <c r="AK24" s="24">
-        <f>+W24/$Y24</f>
+        <f t="shared" si="13"/>
         <v>0.99894955266461494</v>
       </c>
       <c r="AL24" s="24">
-        <f>+X24/$Y24</f>
+        <f t="shared" si="13"/>
         <v>1.050447335385154E-3</v>
       </c>
       <c r="AM24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="1">
         <v>2040</v>
       </c>
@@ -23284,7 +23596,7 @@
         <v>0</v>
       </c>
       <c r="Y25">
-        <f>+SUM(W25:X25)</f>
+        <f t="shared" si="12"/>
         <v>60.496299999999998</v>
       </c>
       <c r="AB25">
@@ -23294,19 +23606,19 @@
         <v>2040</v>
       </c>
       <c r="AK25" s="24">
-        <f>+W25/$Y25</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL25" s="24">
-        <f>+X25/$Y25</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM25">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
         <v>2045</v>
       </c>
@@ -23329,7 +23641,7 @@
         <v>0</v>
       </c>
       <c r="Y26">
-        <f>+SUM(W26:X26)</f>
+        <f t="shared" si="12"/>
         <v>72.998800000000003</v>
       </c>
       <c r="AB26">
@@ -23339,19 +23651,19 @@
         <v>2045</v>
       </c>
       <c r="AK26" s="24">
-        <f>+W26/$Y26</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL26" s="24">
-        <f>+X26/$Y26</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1">
         <v>2050</v>
       </c>
@@ -23374,7 +23686,7 @@
         <v>0</v>
       </c>
       <c r="Y27">
-        <f>+SUM(W27:X27)</f>
+        <f t="shared" si="12"/>
         <v>88.119699999999995</v>
       </c>
       <c r="AB27">
@@ -23384,19 +23696,19 @@
         <v>2050</v>
       </c>
       <c r="AK27" s="24">
-        <f>+W27/$Y27</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL27" s="24">
-        <f>+X27/$Y27</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AM27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>9</v>
       </c>
@@ -23416,7 +23728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="3:39" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:51" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
         <v>0</v>
       </c>
@@ -23450,8 +23762,36 @@
       <c r="AL32" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="AQ32" t="str" cm="1">
+        <f t="array" ref="AQ32:AY34">+TRANSPOSE(AJ32:AL40)</f>
+        <v>Año</v>
+      </c>
+      <c r="AR32">
+        <v>2019</v>
+      </c>
+      <c r="AS32">
+        <v>2020</v>
+      </c>
+      <c r="AT32">
+        <v>2025</v>
+      </c>
+      <c r="AU32">
+        <v>2030</v>
+      </c>
+      <c r="AV32">
+        <v>2035</v>
+      </c>
+      <c r="AW32">
+        <v>2040</v>
+      </c>
+      <c r="AX32">
+        <v>2045</v>
+      </c>
+      <c r="AY32">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="33" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1">
         <v>2019</v>
       </c>
@@ -23489,19 +23829,46 @@
         <v>2019</v>
       </c>
       <c r="AK33" s="24">
-        <f>+W33/$Y33</f>
+        <f t="shared" ref="AK33:AL40" si="15">+W33/$Y33</f>
         <v>0.73862618670258562</v>
       </c>
       <c r="AL33" s="24">
-        <f>+X33/$Y33</f>
+        <f t="shared" si="15"/>
         <v>0.26137381329741433</v>
       </c>
       <c r="AM33">
         <f>+SUM(AK33:AL33)</f>
         <v>1</v>
       </c>
+      <c r="AQ33" t="str">
+        <v>Gas Natural</v>
+      </c>
+      <c r="AR33" s="35">
+        <v>0.73862618670258562</v>
+      </c>
+      <c r="AS33" s="35">
+        <v>0.73714879231338193</v>
+      </c>
+      <c r="AT33" s="35">
+        <v>0.77092060048158928</v>
+      </c>
+      <c r="AU33" s="35">
+        <v>0.77283180112718453</v>
+      </c>
+      <c r="AV33" s="35">
+        <v>0.57300144898651739</v>
+      </c>
+      <c r="AW33" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX33" s="35">
+        <v>0</v>
+      </c>
+      <c r="AY33" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1">
         <v>2020</v>
       </c>
@@ -23527,7 +23894,7 @@
         <v>18.372800000000002</v>
       </c>
       <c r="Y34">
-        <f t="shared" ref="Y34:Y40" si="12">+SUM(W34:X34)</f>
+        <f t="shared" ref="Y34:Y40" si="16">+SUM(W34:X34)</f>
         <v>69.898099999999999</v>
       </c>
       <c r="AB34">
@@ -23537,19 +23904,46 @@
         <v>2020</v>
       </c>
       <c r="AK34" s="24">
-        <f>+W34/$Y34</f>
+        <f t="shared" si="15"/>
         <v>0.73714879231338193</v>
       </c>
       <c r="AL34" s="24">
-        <f>+X34/$Y34</f>
+        <f t="shared" si="15"/>
         <v>0.26285120768661813</v>
       </c>
       <c r="AM34">
-        <f t="shared" ref="AM34:AM40" si="13">+SUM(AK34:AL34)</f>
+        <f t="shared" ref="AM34:AM40" si="17">+SUM(AK34:AL34)</f>
+        <v>1</v>
+      </c>
+      <c r="AQ34" t="str">
+        <v>GLP</v>
+      </c>
+      <c r="AR34" s="35">
+        <v>0.26137381329741433</v>
+      </c>
+      <c r="AS34" s="35">
+        <v>0.26285120768661813</v>
+      </c>
+      <c r="AT34" s="35">
+        <v>0.22907939951841078</v>
+      </c>
+      <c r="AU34" s="35">
+        <v>0.2271681988728155</v>
+      </c>
+      <c r="AV34" s="35">
+        <v>0.42699855101348255</v>
+      </c>
+      <c r="AW34" s="35">
+        <v>1</v>
+      </c>
+      <c r="AX34" s="35">
+        <v>1</v>
+      </c>
+      <c r="AY34" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1">
         <v>2025</v>
       </c>
@@ -23575,7 +23969,7 @@
         <v>14.6127</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>63.788799999999995</v>
       </c>
       <c r="AB35">
@@ -23585,19 +23979,19 @@
         <v>2025</v>
       </c>
       <c r="AK35" s="24">
-        <f>+W35/$Y35</f>
+        <f t="shared" si="15"/>
         <v>0.77092060048158928</v>
       </c>
       <c r="AL35" s="24">
-        <f>+X35/$Y35</f>
+        <f t="shared" si="15"/>
         <v>0.22907939951841078</v>
       </c>
       <c r="AM35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1">
         <v>2030</v>
       </c>
@@ -23623,7 +24017,7 @@
         <v>8.6338000000000008</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>38.0062</v>
       </c>
       <c r="AB36">
@@ -23633,19 +24027,19 @@
         <v>2030</v>
       </c>
       <c r="AK36" s="24">
-        <f>+W36/$Y36</f>
+        <f t="shared" si="15"/>
         <v>0.77283180112718453</v>
       </c>
       <c r="AL36" s="24">
-        <f>+X36/$Y36</f>
+        <f t="shared" si="15"/>
         <v>0.2271681988728155</v>
       </c>
       <c r="AM36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1">
         <v>2035</v>
       </c>
@@ -23671,7 +24065,7 @@
         <v>7.9271000000000003</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>18.564700000000002</v>
       </c>
       <c r="AB37">
@@ -23681,19 +24075,19 @@
         <v>2035</v>
       </c>
       <c r="AK37" s="24">
-        <f>+W37/$Y37</f>
+        <f t="shared" si="15"/>
         <v>0.57300144898651739</v>
       </c>
       <c r="AL37" s="24">
-        <f>+X37/$Y37</f>
+        <f t="shared" si="15"/>
         <v>0.42699855101348255</v>
       </c>
       <c r="AM37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1">
         <v>2040</v>
       </c>
@@ -23719,7 +24113,7 @@
         <v>7.9062000000000001</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>7.9062000000000001</v>
       </c>
       <c r="AB38">
@@ -23729,19 +24123,19 @@
         <v>2040</v>
       </c>
       <c r="AK38" s="24">
-        <f>+W38/$Y38</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AL38" s="24">
-        <f>+X38/$Y38</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AM38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1">
         <v>2045</v>
       </c>
@@ -23767,7 +24161,7 @@
         <v>7.9055999999999997</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>7.9055999999999997</v>
       </c>
       <c r="AB39">
@@ -23777,19 +24171,19 @@
         <v>2045</v>
       </c>
       <c r="AK39" s="24">
-        <f>+W39/$Y39</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AL39" s="24">
-        <f>+X39/$Y39</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AM39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="1">
         <v>2050</v>
       </c>
@@ -23815,7 +24209,7 @@
         <v>7.4988999999999999</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>7.4988999999999999</v>
       </c>
       <c r="AB40">
@@ -23825,19 +24219,19 @@
         <v>2050</v>
       </c>
       <c r="AK40" s="24">
-        <f>+W40/$Y40</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AL40" s="24">
-        <f>+X40/$Y40</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AM40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>19</v>
       </c>
@@ -23857,7 +24251,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="3:45" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:56" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="1" t="s">
         <v>0</v>
       </c>
@@ -23960,8 +24354,36 @@
       <c r="AR47" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="AV47" t="str" cm="1">
+        <f t="array" ref="AV47:BD55">+TRANSPOSE(AJ47:AR55)</f>
+        <v>Año</v>
+      </c>
+      <c r="AW47">
+        <v>2019</v>
+      </c>
+      <c r="AX47">
+        <v>2020</v>
+      </c>
+      <c r="AY47">
+        <v>2025</v>
+      </c>
+      <c r="AZ47">
+        <v>2030</v>
+      </c>
+      <c r="BA47">
+        <v>2035</v>
+      </c>
+      <c r="BB47">
+        <v>2040</v>
+      </c>
+      <c r="BC47">
+        <v>2045</v>
+      </c>
+      <c r="BD47">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="48" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="1">
         <v>2019</v>
       </c>
@@ -24043,7 +24465,7 @@
         <v>0</v>
       </c>
       <c r="AE48">
-        <f t="shared" ref="AE48:AE55" si="14">+SUM(W48:AD48)</f>
+        <f t="shared" ref="AE48:AE55" si="18">+SUM(W48:AD48)</f>
         <v>105.9659</v>
       </c>
       <c r="AG48">
@@ -24053,43 +24475,70 @@
         <v>2019</v>
       </c>
       <c r="AK48" s="24">
-        <f>+W48/$AE48</f>
+        <f t="shared" ref="AK48:AR48" si="19">+W48/$AE48</f>
         <v>2.3815208477444158E-2</v>
       </c>
       <c r="AL48" s="24">
-        <f>+X48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>2.0733084888629265E-3</v>
       </c>
       <c r="AM48" s="24">
-        <f>+Y48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>0.92987932910492899</v>
       </c>
       <c r="AN48" s="24">
-        <f>+Z48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>3.7747992514573081E-5</v>
       </c>
       <c r="AO48" s="24">
-        <f>+AA48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>3.934284519831379E-2</v>
       </c>
       <c r="AP48" s="24">
-        <f>+AB48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>4.1598287751059542E-3</v>
       </c>
       <c r="AQ48" s="24">
-        <f>+AC48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>6.9173196282955177E-4</v>
       </c>
       <c r="AR48" s="24">
-        <f>+AD48/$AE48</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AS48">
-        <f t="shared" ref="AS48:AS55" si="15">+SUM(AK48:AR48)</f>
+        <f t="shared" ref="AS48:AS55" si="20">+SUM(AK48:AR48)</f>
         <v>0.99999999999999989</v>
       </c>
+      <c r="AV48" t="str">
+        <v>Diésel</v>
+      </c>
+      <c r="AW48" s="35">
+        <v>2.3815208477444158E-2</v>
+      </c>
+      <c r="AX48" s="35">
+        <v>2.229784403474367E-2</v>
+      </c>
+      <c r="AY48" s="35">
+        <v>1.3913012996345599E-2</v>
+      </c>
+      <c r="AZ48" s="35">
+        <v>6.2035191203109498E-3</v>
+      </c>
+      <c r="BA48" s="35">
+        <v>4.6787656074508211E-3</v>
+      </c>
+      <c r="BB48" s="35">
+        <v>3.1693536462588964E-3</v>
+      </c>
+      <c r="BC48" s="35">
+        <v>1.7208501930142783E-3</v>
+      </c>
+      <c r="BD48" s="35">
+        <v>1.6342224068375486E-4</v>
+      </c>
     </row>
-    <row r="49" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="1">
         <v>2020</v>
       </c>
@@ -24166,7 +24615,7 @@
         <v>0</v>
       </c>
       <c r="AE49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>98.619399999999999</v>
       </c>
       <c r="AG49">
@@ -24176,43 +24625,70 @@
         <v>2020</v>
       </c>
       <c r="AK49" s="24">
-        <f t="shared" ref="AK49:AK55" si="16">+W49/$AE49</f>
+        <f t="shared" ref="AK49:AK55" si="21">+W49/$AE49</f>
         <v>2.229784403474367E-2</v>
       </c>
       <c r="AL49" s="24">
-        <f>+X49/$AE49</f>
+        <f t="shared" ref="AL49:AR55" si="22">+X49/$AE49</f>
         <v>4.5913887125656819E-3</v>
       </c>
       <c r="AM49" s="24">
-        <f>+Y49/$AE49</f>
+        <f t="shared" si="22"/>
         <v>0.92787524564132418</v>
       </c>
       <c r="AN49" s="24">
-        <f>+Z49/$AE49</f>
+        <f t="shared" si="22"/>
         <v>3.9545971685084271E-5</v>
       </c>
       <c r="AO49" s="24">
-        <f>+AA49/$AE49</f>
+        <f t="shared" si="22"/>
         <v>4.0992948649048767E-2</v>
       </c>
       <c r="AP49" s="24">
-        <f>+AB49/$AE49</f>
+        <f t="shared" si="22"/>
         <v>3.5023534923148995E-3</v>
       </c>
       <c r="AQ49" s="24">
-        <f>+AC49/$AE49</f>
+        <f t="shared" si="22"/>
         <v>7.0067349831777514E-4</v>
       </c>
       <c r="AR49" s="24">
-        <f>+AD49/$AE49</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AS49">
-        <f t="shared" si="15"/>
-        <v>1</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AV49" t="str">
+        <v>Gasolina</v>
+      </c>
+      <c r="AW49" s="35">
+        <v>2.0733084888629265E-3</v>
+      </c>
+      <c r="AX49" s="35">
+        <v>4.5913887125656819E-3</v>
+      </c>
+      <c r="AY49" s="35">
+        <v>3.3783487717883782E-3</v>
+      </c>
+      <c r="AZ49" s="35">
+        <v>1.7902060557512646E-3</v>
+      </c>
+      <c r="BA49" s="35">
+        <v>1.6755816637882767E-3</v>
+      </c>
+      <c r="BB49" s="35">
+        <v>1.6683289082165789E-3</v>
+      </c>
+      <c r="BC49" s="35">
+        <v>1.7261353594547398E-3</v>
+      </c>
+      <c r="BD49" s="35">
+        <v>1.7811611362131437E-3</v>
       </c>
     </row>
-    <row r="50" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="1">
         <v>2025</v>
       </c>
@@ -24289,7 +24765,7 @@
         <v>1.9900000000000001E-2</v>
       </c>
       <c r="AE50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>114.10899999999999</v>
       </c>
       <c r="AG50">
@@ -24299,43 +24775,70 @@
         <v>2025</v>
       </c>
       <c r="AK50" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.3913012996345599E-2</v>
       </c>
       <c r="AL50" s="24">
-        <f>+X50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>3.3783487717883782E-3</v>
       </c>
       <c r="AM50" s="24">
-        <f>+Y50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>0.94452234267235713</v>
       </c>
       <c r="AN50" s="24">
-        <f>+Z50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>2.1908876600443436E-5</v>
       </c>
       <c r="AO50" s="24">
-        <f>+AA50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>3.5195295726016353E-2</v>
       </c>
       <c r="AP50" s="24">
-        <f>+AB50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>2.4651867950818956E-3</v>
       </c>
       <c r="AQ50" s="24">
-        <f>+AC50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>3.2950950407066928E-4</v>
       </c>
       <c r="AR50" s="24">
-        <f>+AD50/$AE50</f>
+        <f t="shared" si="22"/>
         <v>1.7439465773952978E-4</v>
       </c>
       <c r="AS50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.99999999999999989</v>
       </c>
+      <c r="AV50" t="str">
+        <v>Gas Natural</v>
+      </c>
+      <c r="AW50" s="35">
+        <v>0.92987932910492899</v>
+      </c>
+      <c r="AX50" s="35">
+        <v>0.92787524564132418</v>
+      </c>
+      <c r="AY50" s="35">
+        <v>0.94452234267235713</v>
+      </c>
+      <c r="AZ50" s="35">
+        <v>0.80541142879682992</v>
+      </c>
+      <c r="BA50" s="35">
+        <v>0.73652544616169935</v>
+      </c>
+      <c r="BB50" s="35">
+        <v>0.66412745278811813</v>
+      </c>
+      <c r="BC50" s="35">
+        <v>0.65541349028163587</v>
+      </c>
+      <c r="BD50" s="35">
+        <v>0.64728064449587286</v>
+      </c>
     </row>
-    <row r="51" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="1">
         <v>2030</v>
       </c>
@@ -24412,7 +24915,7 @@
         <v>20.510999999999999</v>
       </c>
       <c r="AE51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>131.82839999999999</v>
       </c>
       <c r="AG51">
@@ -24422,43 +24925,70 @@
         <v>2030</v>
       </c>
       <c r="AK51" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>6.2035191203109498E-3</v>
       </c>
       <c r="AL51" s="24">
-        <f>+X51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>1.7902060557512646E-3</v>
       </c>
       <c r="AM51" s="24">
-        <f>+Y51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>0.80541142879682992</v>
       </c>
       <c r="AN51" s="24">
-        <f>+Z51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>6.8270569922717723E-6</v>
       </c>
       <c r="AO51" s="24">
-        <f>+AA51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>2.9614256108698885E-2</v>
       </c>
       <c r="AP51" s="24">
-        <f>+AB51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>1.3851340075431396E-3</v>
       </c>
       <c r="AQ51" s="24">
-        <f>+AC51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR51" s="24">
-        <f>+AD51/$AE51</f>
+        <f t="shared" si="22"/>
         <v>0.15558862885387367</v>
       </c>
       <c r="AS51">
-        <f t="shared" si="15"/>
-        <v>1</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AV51" t="str">
+        <v>Kerosene-Jet</v>
+      </c>
+      <c r="AW51" s="35">
+        <v>3.7747992514573081E-5</v>
+      </c>
+      <c r="AX51" s="35">
+        <v>3.9545971685084271E-5</v>
+      </c>
+      <c r="AY51" s="35">
+        <v>2.1908876600443436E-5</v>
+      </c>
+      <c r="AZ51" s="35">
+        <v>6.8270569922717723E-6</v>
+      </c>
+      <c r="BA51" s="35">
+        <v>6.0930242319573703E-6</v>
+      </c>
+      <c r="BB51" s="35">
+        <v>5.3018927167899754E-6</v>
+      </c>
+      <c r="BC51" s="35">
+        <v>4.7566497964153876E-6</v>
+      </c>
+      <c r="BD51" s="35">
+        <v>4.2386171935267829E-6</v>
       </c>
     </row>
-    <row r="52" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="1">
         <v>2035</v>
       </c>
@@ -24535,7 +25065,7 @@
         <v>33.819299999999998</v>
       </c>
       <c r="AE52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>147.7099</v>
       </c>
       <c r="AG52">
@@ -24545,43 +25075,70 @@
         <v>2035</v>
       </c>
       <c r="AK52" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>4.6787656074508211E-3</v>
       </c>
       <c r="AL52" s="24">
-        <f>+X52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>1.6755816637882767E-3</v>
       </c>
       <c r="AM52" s="24">
-        <f>+Y52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>0.73652544616169935</v>
       </c>
       <c r="AN52" s="24">
-        <f>+Z52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>6.0930242319573703E-6</v>
       </c>
       <c r="AO52" s="24">
-        <f>+AA52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>2.6784934523684599E-2</v>
       </c>
       <c r="AP52" s="24">
-        <f>+AB52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>1.3716074548828481E-3</v>
       </c>
       <c r="AQ52" s="24">
-        <f>+AC52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR52" s="24">
-        <f>+AD52/$AE52</f>
+        <f t="shared" si="22"/>
         <v>0.22895757156426208</v>
       </c>
       <c r="AS52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.99999999999999989</v>
       </c>
+      <c r="AV52" t="str">
+        <v>GLP</v>
+      </c>
+      <c r="AW52" s="35">
+        <v>3.934284519831379E-2</v>
+      </c>
+      <c r="AX52" s="35">
+        <v>4.0992948649048767E-2</v>
+      </c>
+      <c r="AY52" s="35">
+        <v>3.5195295726016353E-2</v>
+      </c>
+      <c r="AZ52" s="35">
+        <v>2.9614256108698885E-2</v>
+      </c>
+      <c r="BA52" s="35">
+        <v>2.6784934523684599E-2</v>
+      </c>
+      <c r="BB52" s="35">
+        <v>2.3821403976537359E-2</v>
+      </c>
+      <c r="BC52" s="35">
+        <v>2.1926041494898754E-2</v>
+      </c>
+      <c r="BD52" s="35">
+        <v>2.0125425392331111E-2</v>
+      </c>
     </row>
-    <row r="53" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="1">
         <v>2040</v>
       </c>
@@ -24658,7 +25215,7 @@
         <v>51.9163</v>
       </c>
       <c r="AE53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>169.75069999999999</v>
       </c>
       <c r="AG53">
@@ -24668,43 +25225,70 @@
         <v>2040</v>
       </c>
       <c r="AK53" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>3.1693536462588964E-3</v>
       </c>
       <c r="AL53" s="24">
-        <f>+X53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>1.6683289082165789E-3</v>
       </c>
       <c r="AM53" s="24">
-        <f>+Y53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>0.66412745278811813</v>
       </c>
       <c r="AN53" s="24">
-        <f>+Z53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>5.3018927167899754E-6</v>
       </c>
       <c r="AO53" s="24">
-        <f>+AA53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>2.3821403976537359E-2</v>
       </c>
       <c r="AP53" s="24">
-        <f>+AB53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>1.369655618504077E-3</v>
       </c>
       <c r="AQ53" s="24">
-        <f>+AC53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR53" s="24">
-        <f>+AD53/$AE53</f>
+        <f t="shared" si="22"/>
         <v>0.30583850316964822</v>
       </c>
       <c r="AS53">
-        <f t="shared" si="15"/>
-        <v>1</v>
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AV53" t="str">
+        <v>Fuel Oil</v>
+      </c>
+      <c r="AW53" s="35">
+        <v>4.1598287751059542E-3</v>
+      </c>
+      <c r="AX53" s="35">
+        <v>3.5023534923148995E-3</v>
+      </c>
+      <c r="AY53" s="35">
+        <v>2.4651867950818956E-3</v>
+      </c>
+      <c r="AZ53" s="35">
+        <v>1.3851340075431396E-3</v>
+      </c>
+      <c r="BA53" s="35">
+        <v>1.3716074548828481E-3</v>
+      </c>
+      <c r="BB53" s="35">
+        <v>1.369655618504077E-3</v>
+      </c>
+      <c r="BC53" s="35">
+        <v>1.4185386726198782E-3</v>
+      </c>
+      <c r="BD53" s="35">
+        <v>1.4651486765624247E-3</v>
       </c>
     </row>
-    <row r="54" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="1">
         <v>2045</v>
       </c>
@@ -24781,7 +25365,7 @@
         <v>60.128700000000002</v>
       </c>
       <c r="AE54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>189.20880000000002</v>
       </c>
       <c r="AG54">
@@ -24791,43 +25375,70 @@
         <v>2045</v>
       </c>
       <c r="AK54" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.7208501930142783E-3</v>
       </c>
       <c r="AL54" s="24">
-        <f>+X54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>1.7261353594547398E-3</v>
       </c>
       <c r="AM54" s="24">
-        <f>+Y54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>0.65541349028163587</v>
       </c>
       <c r="AN54" s="24">
-        <f>+Z54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>4.7566497964153876E-6</v>
       </c>
       <c r="AO54" s="24">
-        <f>+AA54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>2.1926041494898754E-2</v>
       </c>
       <c r="AP54" s="24">
-        <f>+AB54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>1.4185386726198782E-3</v>
       </c>
       <c r="AQ54" s="24">
-        <f>+AC54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR54" s="24">
-        <f>+AD54/$AE54</f>
+        <f t="shared" si="22"/>
         <v>0.31779018734857994</v>
       </c>
       <c r="AS54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.99999999999999978</v>
       </c>
+      <c r="AV54" t="str">
+        <v>Petróleo</v>
+      </c>
+      <c r="AW54" s="35">
+        <v>6.9173196282955177E-4</v>
+      </c>
+      <c r="AX54" s="35">
+        <v>7.0067349831777514E-4</v>
+      </c>
+      <c r="AY54" s="35">
+        <v>3.2950950407066928E-4</v>
+      </c>
+      <c r="AZ54" s="35">
+        <v>0</v>
+      </c>
+      <c r="BA54" s="35">
+        <v>0</v>
+      </c>
+      <c r="BB54" s="35">
+        <v>0</v>
+      </c>
+      <c r="BC54" s="35">
+        <v>0</v>
+      </c>
+      <c r="BD54" s="35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="1">
         <v>2050</v>
       </c>
@@ -24904,7 +25515,7 @@
         <v>69.895899999999997</v>
       </c>
       <c r="AE55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>212.33340000000004</v>
       </c>
       <c r="AG55">
@@ -24914,44 +25525,71 @@
         <v>2050</v>
       </c>
       <c r="AK55" s="24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>1.6342224068375486E-4</v>
       </c>
       <c r="AL55" s="24">
-        <f>+X55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>1.7811611362131437E-3</v>
       </c>
       <c r="AM55" s="24">
-        <f>+Y55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>0.64728064449587286</v>
       </c>
       <c r="AN55" s="24">
-        <f>+Z55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>4.2386171935267829E-6</v>
       </c>
       <c r="AO55" s="24">
-        <f>+AA55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>2.0125425392331111E-2</v>
       </c>
       <c r="AP55" s="24">
-        <f>+AB55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>1.4651486765624247E-3</v>
       </c>
       <c r="AQ55" s="24">
-        <f>+AC55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR55" s="24">
-        <f>+AD55/$AE55</f>
+        <f t="shared" si="22"/>
         <v>0.32917995944114298</v>
       </c>
       <c r="AS55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>0.99999999999999978</v>
       </c>
+      <c r="AV55" t="str">
+        <v>Hidrógeno</v>
+      </c>
+      <c r="AW55" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX55" s="35">
+        <v>0</v>
+      </c>
+      <c r="AY55" s="35">
+        <v>1.7439465773952978E-4</v>
+      </c>
+      <c r="AZ55" s="35">
+        <v>0.15558862885387367</v>
+      </c>
+      <c r="BA55" s="35">
+        <v>0.22895757156426208</v>
+      </c>
+      <c r="BB55" s="35">
+        <v>0.30583850316964822</v>
+      </c>
+      <c r="BC55" s="35">
+        <v>0.31779018734857994</v>
+      </c>
+      <c r="BD55" s="35">
+        <v>0.32917995944114298</v>
+      </c>
     </row>
-    <row r="61" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="1" t="s">
         <v>21</v>
       </c>
@@ -24994,8 +25632,36 @@
       <c r="AQ62" s="1"/>
       <c r="AR62" s="1"/>
       <c r="AS62" s="1"/>
+      <c r="AV62" t="str" cm="1">
+        <f t="array" ref="AV62:BD70">+TRANSPOSE(AJ63:AR71)</f>
+        <v>Año</v>
+      </c>
+      <c r="AW62">
+        <v>2019</v>
+      </c>
+      <c r="AX62">
+        <v>2020</v>
+      </c>
+      <c r="AY62">
+        <v>2025</v>
+      </c>
+      <c r="AZ62">
+        <v>2030</v>
+      </c>
+      <c r="BA62">
+        <v>2035</v>
+      </c>
+      <c r="BB62">
+        <v>2040</v>
+      </c>
+      <c r="BC62">
+        <v>2045</v>
+      </c>
+      <c r="BD62">
+        <v>2050</v>
+      </c>
     </row>
-    <row r="63" spans="3:45" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:56" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="1" t="s">
         <v>0</v>
       </c>
@@ -25080,8 +25746,35 @@
       <c r="AR63" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="AV63" t="str">
+        <v>Diésel</v>
+      </c>
+      <c r="AW63" s="35">
+        <v>0.42556332971371874</v>
+      </c>
+      <c r="AX63" s="35">
+        <v>0.43875733275414347</v>
+      </c>
+      <c r="AY63" s="35">
+        <v>0.45035521330209333</v>
+      </c>
+      <c r="AZ63" s="35">
+        <v>0.46181170845465164</v>
+      </c>
+      <c r="BA63" s="35">
+        <v>0.45939877241954008</v>
+      </c>
+      <c r="BB63" s="35">
+        <v>0.43014861144267835</v>
+      </c>
+      <c r="BC63" s="35">
+        <v>0.37486176266182086</v>
+      </c>
+      <c r="BD63" s="35">
+        <v>0.30944250942847534</v>
+      </c>
     </row>
-    <row r="64" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="1">
         <v>2019</v>
       </c>
@@ -25142,7 +25835,7 @@
         <v>0</v>
       </c>
       <c r="AE64">
-        <f t="shared" ref="AE64:AE71" si="17">+SUM(W64:AD64)</f>
+        <f t="shared" ref="AE64:AE71" si="23">+SUM(W64:AD64)</f>
         <v>574.73889999999994</v>
       </c>
       <c r="AG64">
@@ -25152,43 +25845,70 @@
         <v>2019</v>
       </c>
       <c r="AK64" s="24">
-        <f>+W64/$AE64</f>
+        <f t="shared" ref="AK64:AR64" si="24">+W64/$AE64</f>
         <v>0.42556332971371874</v>
       </c>
       <c r="AL64" s="24">
-        <f>+X64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>0.43290649023408723</v>
       </c>
       <c r="AM64" s="24">
-        <f>+Y64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>3.638539169699493E-2</v>
       </c>
       <c r="AN64" s="24">
-        <f>+Z64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>0.10288236971605716</v>
       </c>
       <c r="AO64" s="24">
-        <f>+AA64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>5.4111527860738156E-5</v>
       </c>
       <c r="AP64" s="24">
-        <f>+AB64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>1.2957188037907301E-3</v>
       </c>
       <c r="AQ64" s="24">
-        <f>+AC64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>9.1258830749058398E-4</v>
       </c>
       <c r="AR64" s="24">
-        <f>+AD64/$AE64</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AS64">
-        <f t="shared" ref="AS64:AS71" si="18">+SUM(AK64:AR64)</f>
+        <f t="shared" ref="AS64:AS71" si="25">+SUM(AK64:AR64)</f>
         <v>1.0000000000000002</v>
       </c>
+      <c r="AV64" t="str">
+        <v>Gasolina</v>
+      </c>
+      <c r="AW64" s="35">
+        <v>0.43290649023408723</v>
+      </c>
+      <c r="AX64" s="35">
+        <v>0.44296269507607156</v>
+      </c>
+      <c r="AY64" s="35">
+        <v>0.42561381092951567</v>
+      </c>
+      <c r="AZ64" s="35">
+        <v>0.39230830185162452</v>
+      </c>
+      <c r="BA64" s="35">
+        <v>0.34082498701456904</v>
+      </c>
+      <c r="BB64" s="35">
+        <v>0.27406242928687291</v>
+      </c>
+      <c r="BC64" s="35">
+        <v>0.20805142683391364</v>
+      </c>
+      <c r="BD64" s="35">
+        <v>0.14687318137688032</v>
+      </c>
     </row>
-    <row r="65" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="1">
         <v>2020</v>
       </c>
@@ -25247,7 +25967,7 @@
         <v>6.4000000000000003E-3</v>
       </c>
       <c r="AE65">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>577.35809999999992</v>
       </c>
       <c r="AG65">
@@ -25257,43 +25977,70 @@
         <v>2020</v>
       </c>
       <c r="AK65" s="24">
-        <f t="shared" ref="AK65:AK71" si="19">+W65/$AE65</f>
+        <f t="shared" ref="AK65:AK71" si="26">+W65/$AE65</f>
         <v>0.43875733275414347</v>
       </c>
       <c r="AL65" s="24">
-        <f>+X65/$AE65</f>
+        <f t="shared" ref="AL65:AR71" si="27">+X65/$AE65</f>
         <v>0.44296269507607156</v>
       </c>
       <c r="AM65" s="24">
-        <f>+Y65/$AE65</f>
+        <f t="shared" si="27"/>
         <v>3.4769755546860785E-2</v>
       </c>
       <c r="AN65" s="24">
-        <f>+Z65/$AE65</f>
+        <f t="shared" si="27"/>
         <v>8.1887480231073229E-2</v>
       </c>
       <c r="AO65" s="24">
-        <f>+AA65/$AE65</f>
+        <f t="shared" si="27"/>
         <v>5.2826833121419799E-5</v>
       </c>
       <c r="AP65" s="24">
-        <f>+AB65/$AE65</f>
+        <f t="shared" si="27"/>
         <v>1.5588245839107482E-3</v>
       </c>
       <c r="AQ65" s="24">
-        <f>+AC65/$AE65</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR65" s="24">
-        <f>+AD65/$AE65</f>
+        <f t="shared" si="27"/>
         <v>1.1084974818920876E-5</v>
       </c>
       <c r="AS65">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1.0000000000000002</v>
       </c>
+      <c r="AV65" t="str">
+        <v>Gas Natural</v>
+      </c>
+      <c r="AW65" s="35">
+        <v>3.638539169699493E-2</v>
+      </c>
+      <c r="AX65" s="35">
+        <v>3.4769755546860785E-2</v>
+      </c>
+      <c r="AY65" s="35">
+        <v>2.6206088904079453E-2</v>
+      </c>
+      <c r="AZ65" s="35">
+        <v>2.5353871240987615E-2</v>
+      </c>
+      <c r="BA65" s="35">
+        <v>3.9295538881349151E-2</v>
+      </c>
+      <c r="BB65" s="35">
+        <v>7.5994452374206489E-2</v>
+      </c>
+      <c r="BC65" s="35">
+        <v>0.12796123546939814</v>
+      </c>
+      <c r="BD65" s="35">
+        <v>0.1826924856020033</v>
+      </c>
     </row>
-    <row r="66" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="1">
         <v>2025</v>
       </c>
@@ -25352,7 +26099,7 @@
         <v>0.18429999999999999</v>
       </c>
       <c r="AE66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>605.93169999999998</v>
       </c>
       <c r="AG66">
@@ -25362,43 +26109,70 @@
         <v>2025</v>
       </c>
       <c r="AK66" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.45035521330209333</v>
       </c>
       <c r="AL66" s="24">
-        <f>+X66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>0.42561381092951567</v>
       </c>
       <c r="AM66" s="24">
-        <f>+Y66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>2.6206088904079453E-2</v>
       </c>
       <c r="AN66" s="24">
-        <f>+Z66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>9.5640482252372677E-2</v>
       </c>
       <c r="AO66" s="24">
-        <f>+AA66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>5.9577671872919011E-5</v>
       </c>
       <c r="AP66" s="24">
-        <f>+AB66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>1.8206672468200624E-3</v>
       </c>
       <c r="AQ66" s="24">
-        <f>+AC66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR66" s="24">
-        <f>+AD66/$AE66</f>
+        <f t="shared" si="27"/>
         <v>3.0415969324595497E-4</v>
       </c>
       <c r="AS66">
-        <f t="shared" si="18"/>
-        <v>1</v>
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="AV66" t="str">
+        <v>Kerosene-Jet</v>
+      </c>
+      <c r="AW66" s="35">
+        <v>0.10288236971605716</v>
+      </c>
+      <c r="AX66" s="35">
+        <v>8.1887480231073229E-2</v>
+      </c>
+      <c r="AY66" s="35">
+        <v>9.5640482252372677E-2</v>
+      </c>
+      <c r="AZ66" s="35">
+        <v>0.11505236282677034</v>
+      </c>
+      <c r="BA66" s="35">
+        <v>0.14099923763228084</v>
+      </c>
+      <c r="BB66" s="35">
+        <v>0.17160508275369818</v>
+      </c>
+      <c r="BC66" s="35">
+        <v>0.20881799377728014</v>
+      </c>
+      <c r="BD66" s="35">
+        <v>0.24927097977595086</v>
       </c>
     </row>
-    <row r="67" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="1">
         <v>2030</v>
       </c>
@@ -25457,7 +26231,7 @@
         <v>1.9153</v>
       </c>
       <c r="AE67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>601.9633</v>
       </c>
       <c r="AG67">
@@ -25467,43 +26241,70 @@
         <v>2030</v>
       </c>
       <c r="AK67" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.46181170845465164</v>
       </c>
       <c r="AL67" s="24">
-        <f>+X67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>0.39230830185162452</v>
       </c>
       <c r="AM67" s="24">
-        <f>+Y67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>2.5353871240987615E-2</v>
       </c>
       <c r="AN67" s="24">
-        <f>+Z67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>0.11505236282677034</v>
       </c>
       <c r="AO67" s="24">
-        <f>+AA67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>1.0183345064391799E-4</v>
       </c>
       <c r="AP67" s="24">
-        <f>+AB67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>2.1901667427233519E-3</v>
       </c>
       <c r="AQ67" s="24">
-        <f>+AC67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR67" s="24">
-        <f>+AD67/$AE67</f>
+        <f t="shared" si="27"/>
         <v>3.1817554325986319E-3</v>
       </c>
       <c r="AS67">
-        <f t="shared" si="18"/>
-        <v>1</v>
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="AV67" t="str">
+        <v>GLP</v>
+      </c>
+      <c r="AW67" s="35">
+        <v>5.4111527860738156E-5</v>
+      </c>
+      <c r="AX67" s="35">
+        <v>5.2826833121419799E-5</v>
+      </c>
+      <c r="AY67" s="35">
+        <v>5.9577671872919011E-5</v>
+      </c>
+      <c r="AZ67" s="35">
+        <v>1.0183345064391799E-4</v>
+      </c>
+      <c r="BA67" s="35">
+        <v>3.5047478274391469E-4</v>
+      </c>
+      <c r="BB67" s="35">
+        <v>9.630382430420878E-4</v>
+      </c>
+      <c r="BC67" s="35">
+        <v>1.7366627616025936E-3</v>
+      </c>
+      <c r="BD67" s="35">
+        <v>2.5366028722332056E-3</v>
       </c>
     </row>
-    <row r="68" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="1">
         <v>2035</v>
       </c>
@@ -25562,7 +26363,7 @@
         <v>9.6670999999999996</v>
       </c>
       <c r="AE68">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>587.77409999999998</v>
       </c>
       <c r="AG68">
@@ -25572,43 +26373,70 @@
         <v>2035</v>
       </c>
       <c r="AK68" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.45939877241954008</v>
       </c>
       <c r="AL68" s="24">
-        <f>+X68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>0.34082498701456904</v>
       </c>
       <c r="AM68" s="24">
-        <f>+Y68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>3.9295538881349151E-2</v>
       </c>
       <c r="AN68" s="24">
-        <f>+Z68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>0.14099923763228084</v>
       </c>
       <c r="AO68" s="24">
-        <f>+AA68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>3.5047478274391469E-4</v>
       </c>
       <c r="AP68" s="24">
-        <f>+AB68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>2.6840243556155332E-3</v>
       </c>
       <c r="AQ68" s="24">
-        <f>+AC68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR68" s="24">
-        <f>+AD68/$AE68</f>
+        <f t="shared" si="27"/>
         <v>1.6446964913901446E-2</v>
       </c>
       <c r="AS68">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>0.99999999999999989</v>
       </c>
+      <c r="AV68" t="str">
+        <v>Fuel Oil</v>
+      </c>
+      <c r="AW68" s="35">
+        <v>1.2957188037907301E-3</v>
+      </c>
+      <c r="AX68" s="35">
+        <v>1.5588245839107482E-3</v>
+      </c>
+      <c r="AY68" s="35">
+        <v>1.8206672468200624E-3</v>
+      </c>
+      <c r="AZ68" s="35">
+        <v>2.1901667427233519E-3</v>
+      </c>
+      <c r="BA68" s="35">
+        <v>2.6840243556155332E-3</v>
+      </c>
+      <c r="BB68" s="35">
+        <v>3.2666547619397469E-3</v>
+      </c>
+      <c r="BC68" s="35">
+        <v>3.9751294733146453E-3</v>
+      </c>
+      <c r="BD68" s="35">
+        <v>4.74504627572168E-3</v>
+      </c>
     </row>
-    <row r="69" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="1">
         <v>2040</v>
       </c>
@@ -25667,7 +26495,7 @@
         <v>25.4299</v>
       </c>
       <c r="AE69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>578.48169999999993</v>
       </c>
       <c r="AG69">
@@ -25677,43 +26505,70 @@
         <v>2040</v>
       </c>
       <c r="AK69" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.43014861144267835</v>
       </c>
       <c r="AL69" s="24">
-        <f>+X69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>0.27406242928687291</v>
       </c>
       <c r="AM69" s="24">
-        <f>+Y69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>7.5994452374206489E-2</v>
       </c>
       <c r="AN69" s="24">
-        <f>+Z69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>0.17160508275369818</v>
       </c>
       <c r="AO69" s="24">
-        <f>+AA69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>9.630382430420878E-4</v>
       </c>
       <c r="AP69" s="24">
-        <f>+AB69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>3.2666547619397469E-3</v>
       </c>
       <c r="AQ69" s="24">
-        <f>+AC69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR69" s="24">
-        <f>+AD69/$AE69</f>
+        <f t="shared" si="27"/>
         <v>4.3959731137562352E-2</v>
       </c>
       <c r="AS69">
-        <f t="shared" si="18"/>
-        <v>1</v>
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="AV69" t="str">
+        <v>AVGAS</v>
+      </c>
+      <c r="AW69" s="35">
+        <v>9.1258830749058398E-4</v>
+      </c>
+      <c r="AX69" s="35">
+        <v>0</v>
+      </c>
+      <c r="AY69" s="35">
+        <v>0</v>
+      </c>
+      <c r="AZ69" s="35">
+        <v>0</v>
+      </c>
+      <c r="BA69" s="35">
+        <v>0</v>
+      </c>
+      <c r="BB69" s="35">
+        <v>0</v>
+      </c>
+      <c r="BC69" s="35">
+        <v>0</v>
+      </c>
+      <c r="BD69" s="35">
+        <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C70" s="1">
         <v>2045</v>
       </c>
@@ -25772,7 +26627,7 @@
         <v>42.5154</v>
       </c>
       <c r="AE70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>569.94369999999992</v>
       </c>
       <c r="AG70">
@@ -25782,43 +26637,70 @@
         <v>2045</v>
       </c>
       <c r="AK70" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.37486176266182086</v>
       </c>
       <c r="AL70" s="24">
-        <f>+X70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>0.20805142683391364</v>
       </c>
       <c r="AM70" s="24">
-        <f>+Y70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>0.12796123546939814</v>
       </c>
       <c r="AN70" s="24">
-        <f>+Z70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>0.20881799377728014</v>
       </c>
       <c r="AO70" s="24">
-        <f>+AA70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>1.7366627616025936E-3</v>
       </c>
       <c r="AP70" s="24">
-        <f>+AB70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>3.9751294733146453E-3</v>
       </c>
       <c r="AQ70" s="24">
-        <f>+AC70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR70" s="24">
-        <f>+AD70/$AE70</f>
+        <f t="shared" si="27"/>
         <v>7.4595789022670139E-2</v>
       </c>
       <c r="AS70">
-        <f t="shared" si="18"/>
+        <f t="shared" si="25"/>
         <v>1.0000000000000002</v>
       </c>
+      <c r="AV70" t="str">
+        <v>Hidrógeno</v>
+      </c>
+      <c r="AW70" s="35">
+        <v>0</v>
+      </c>
+      <c r="AX70" s="35">
+        <v>1.1084974818920876E-5</v>
+      </c>
+      <c r="AY70" s="35">
+        <v>3.0415969324595497E-4</v>
+      </c>
+      <c r="AZ70" s="35">
+        <v>3.1817554325986319E-3</v>
+      </c>
+      <c r="BA70" s="35">
+        <v>1.6446964913901446E-2</v>
+      </c>
+      <c r="BB70" s="35">
+        <v>4.3959731137562352E-2</v>
+      </c>
+      <c r="BC70" s="35">
+        <v>7.4595789022670139E-2</v>
+      </c>
+      <c r="BD70" s="35">
+        <v>0.10443919466873523</v>
+      </c>
     </row>
-    <row r="71" spans="3:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="1">
         <v>2050</v>
       </c>
@@ -25877,7 +26759,7 @@
         <v>59.8324</v>
       </c>
       <c r="AE71">
-        <f t="shared" si="17"/>
+        <f t="shared" si="23"/>
         <v>572.8922</v>
       </c>
       <c r="AG71">
@@ -25887,40 +26769,676 @@
         <v>2050</v>
       </c>
       <c r="AK71" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>0.30944250942847534</v>
       </c>
       <c r="AL71" s="24">
-        <f>+X71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>0.14687318137688032</v>
       </c>
       <c r="AM71" s="24">
-        <f>+Y71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>0.1826924856020033</v>
       </c>
       <c r="AN71" s="24">
-        <f>+Z71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>0.24927097977595086</v>
       </c>
       <c r="AO71" s="24">
-        <f>+AA71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>2.5366028722332056E-3</v>
       </c>
       <c r="AP71" s="24">
-        <f>+AB71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>4.74504627572168E-3</v>
       </c>
       <c r="AQ71" s="24">
-        <f>+AC71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AR71" s="24">
-        <f>+AD71/$AE71</f>
+        <f t="shared" si="27"/>
         <v>0.10443919466873523</v>
       </c>
       <c r="AS71">
-        <f t="shared" si="18"/>
-        <v>1</v>
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V110" t="s">
+        <v>19</v>
+      </c>
+      <c r="W110" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V111" t="s">
+        <v>0</v>
+      </c>
+      <c r="W111" t="s">
+        <v>1</v>
+      </c>
+      <c r="X111" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y111" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z111" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA111" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB111" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC111" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD111" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="112" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V112">
+        <v>2019</v>
+      </c>
+      <c r="W112">
+        <v>2.5236000000000001</v>
+      </c>
+      <c r="X112">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="Y112">
+        <v>98.535499999999999</v>
+      </c>
+      <c r="Z112">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AA112">
+        <v>4.1689999999999996</v>
+      </c>
+      <c r="AB112">
+        <v>0.44080000000000003</v>
+      </c>
+      <c r="AC112">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="AD112">
+        <v>0</v>
+      </c>
+      <c r="AE112">
+        <v>105.9659</v>
+      </c>
+      <c r="AG112">
+        <v>105.9659</v>
+      </c>
+    </row>
+    <row r="113" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V113">
+        <v>2020</v>
+      </c>
+      <c r="W113">
+        <v>2.1989999999999998</v>
+      </c>
+      <c r="X113">
+        <v>0.45279999999999998</v>
+      </c>
+      <c r="Y113">
+        <v>91.506500000000003</v>
+      </c>
+      <c r="Z113">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="AA113">
+        <v>4.0427</v>
+      </c>
+      <c r="AB113">
+        <v>0.34539999999999998</v>
+      </c>
+      <c r="AC113">
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="AD113">
+        <v>0</v>
+      </c>
+      <c r="AE113">
+        <v>98.619399999999999</v>
+      </c>
+      <c r="AG113">
+        <v>98.619399999999999</v>
+      </c>
+    </row>
+    <row r="114" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V114">
+        <v>2025</v>
+      </c>
+      <c r="W114">
+        <v>1.5875999999999999</v>
+      </c>
+      <c r="X114">
+        <v>0.38550000000000001</v>
+      </c>
+      <c r="Y114">
+        <v>107.77849999999999</v>
+      </c>
+      <c r="Z114">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AA114">
+        <v>4.0160999999999998</v>
+      </c>
+      <c r="AB114">
+        <v>0.28129999999999999</v>
+      </c>
+      <c r="AC114">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="AD114">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="AE114">
+        <v>114.10899999999999</v>
+      </c>
+      <c r="AG114">
+        <v>114.10899999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V115">
+        <v>2030</v>
+      </c>
+      <c r="W115">
+        <v>0.81779999999999997</v>
+      </c>
+      <c r="X115">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="Y115">
+        <v>106.17610000000001</v>
+      </c>
+      <c r="Z115">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AA115">
+        <v>3.9039999999999999</v>
+      </c>
+      <c r="AB115">
+        <v>0.18260000000000001</v>
+      </c>
+      <c r="AC115">
+        <v>0</v>
+      </c>
+      <c r="AD115">
+        <v>20.510999999999999</v>
+      </c>
+      <c r="AE115">
+        <v>131.82839999999999</v>
+      </c>
+      <c r="AG115">
+        <v>131.82839999999999</v>
+      </c>
+    </row>
+    <row r="116" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V116">
+        <v>2035</v>
+      </c>
+      <c r="W116">
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="X116">
+        <v>0.2475</v>
+      </c>
+      <c r="Y116">
+        <v>108.7921</v>
+      </c>
+      <c r="Z116">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AA116">
+        <v>3.9563999999999999</v>
+      </c>
+      <c r="AB116">
+        <v>0.2026</v>
+      </c>
+      <c r="AC116">
+        <v>0</v>
+      </c>
+      <c r="AD116">
+        <v>33.819299999999998</v>
+      </c>
+      <c r="AE116">
+        <v>147.7099</v>
+      </c>
+      <c r="AG116">
+        <v>147.7099</v>
+      </c>
+    </row>
+    <row r="117" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V117">
+        <v>2040</v>
+      </c>
+      <c r="W117">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="X117">
+        <v>0.28320000000000001</v>
+      </c>
+      <c r="Y117">
+        <v>112.73609999999999</v>
+      </c>
+      <c r="Z117">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AA117">
+        <v>4.0437000000000003</v>
+      </c>
+      <c r="AB117">
+        <v>0.23250000000000001</v>
+      </c>
+      <c r="AC117">
+        <v>0</v>
+      </c>
+      <c r="AD117">
+        <v>51.9163</v>
+      </c>
+      <c r="AE117">
+        <v>169.75069999999999</v>
+      </c>
+      <c r="AG117">
+        <v>169.75069999999999</v>
+      </c>
+    </row>
+    <row r="118" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V118">
+        <v>2045</v>
+      </c>
+      <c r="W118">
+        <v>0.3256</v>
+      </c>
+      <c r="X118">
+        <v>0.3266</v>
+      </c>
+      <c r="Y118">
+        <v>124.01</v>
+      </c>
+      <c r="Z118">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AA118">
+        <v>4.1486000000000001</v>
+      </c>
+      <c r="AB118">
+        <v>0.26840000000000003</v>
+      </c>
+      <c r="AC118">
+        <v>0</v>
+      </c>
+      <c r="AD118">
+        <v>60.128700000000002</v>
+      </c>
+      <c r="AE118">
+        <v>189.20880000000002</v>
+      </c>
+      <c r="AG118">
+        <v>189.20880000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V119">
+        <v>2050</v>
+      </c>
+      <c r="W119">
+        <v>3.4700000000000002E-2</v>
+      </c>
+      <c r="X119">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="Y119">
+        <v>137.4393</v>
+      </c>
+      <c r="Z119">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AA119">
+        <v>4.2732999999999999</v>
+      </c>
+      <c r="AB119">
+        <v>0.31109999999999999</v>
+      </c>
+      <c r="AC119">
+        <v>0</v>
+      </c>
+      <c r="AD119">
+        <v>69.895899999999997</v>
+      </c>
+      <c r="AE119">
+        <v>212.33340000000004</v>
+      </c>
+      <c r="AG119">
+        <v>212.33340000000004</v>
+      </c>
+    </row>
+    <row r="122" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V122" t="s">
+        <v>19</v>
+      </c>
+      <c r="W122" t="s">
+        <v>0</v>
+      </c>
+      <c r="X122">
+        <v>2019</v>
+      </c>
+      <c r="Y122">
+        <v>2020</v>
+      </c>
+      <c r="Z122">
+        <v>2025</v>
+      </c>
+      <c r="AA122">
+        <v>2030</v>
+      </c>
+      <c r="AB122">
+        <v>2035</v>
+      </c>
+      <c r="AC122">
+        <v>2040</v>
+      </c>
+      <c r="AD122">
+        <v>2045</v>
+      </c>
+      <c r="AE122">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="123" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="V123" t="s">
+        <v>23</v>
+      </c>
+      <c r="W123" t="s">
+        <v>1</v>
+      </c>
+      <c r="X123">
+        <v>2.5236000000000001</v>
+      </c>
+      <c r="Y123">
+        <v>2.1989999999999998</v>
+      </c>
+      <c r="Z123">
+        <v>1.5875999999999999</v>
+      </c>
+      <c r="AA123">
+        <v>0.81779999999999997</v>
+      </c>
+      <c r="AB123">
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="AC123">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="AD123">
+        <v>0.3256</v>
+      </c>
+      <c r="AE123">
+        <v>3.4700000000000002E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="W124" t="s">
+        <v>2</v>
+      </c>
+      <c r="X124">
+        <v>0.21970000000000001</v>
+      </c>
+      <c r="Y124">
+        <v>0.45279999999999998</v>
+      </c>
+      <c r="Z124">
+        <v>0.38550000000000001</v>
+      </c>
+      <c r="AA124">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="AB124">
+        <v>0.2475</v>
+      </c>
+      <c r="AC124">
+        <v>0.28320000000000001</v>
+      </c>
+      <c r="AD124">
+        <v>0.3266</v>
+      </c>
+      <c r="AE124">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="125" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="W125" t="s">
+        <v>4</v>
+      </c>
+      <c r="X125">
+        <v>98.535499999999999</v>
+      </c>
+      <c r="Y125">
+        <v>91.506500000000003</v>
+      </c>
+      <c r="Z125">
+        <v>107.77849999999999</v>
+      </c>
+      <c r="AA125">
+        <v>106.17610000000001</v>
+      </c>
+      <c r="AB125">
+        <v>108.7921</v>
+      </c>
+      <c r="AC125">
+        <v>112.73609999999999</v>
+      </c>
+      <c r="AD125">
+        <v>124.01</v>
+      </c>
+      <c r="AE125">
+        <v>137.4393</v>
+      </c>
+    </row>
+    <row r="126" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="W126" t="s">
+        <v>10</v>
+      </c>
+      <c r="X126">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Y126">
+        <v>3.8999999999999998E-3</v>
+      </c>
+      <c r="Z126">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="AA126">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AB126">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AC126">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AD126">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AE126">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="127" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="W127" t="s">
+        <v>7</v>
+      </c>
+      <c r="X127">
+        <v>4.1689999999999996</v>
+      </c>
+      <c r="Y127">
+        <v>4.0427</v>
+      </c>
+      <c r="Z127">
+        <v>4.0160999999999998</v>
+      </c>
+      <c r="AA127">
+        <v>3.9039999999999999</v>
+      </c>
+      <c r="AB127">
+        <v>3.9563999999999999</v>
+      </c>
+      <c r="AC127">
+        <v>4.0437000000000003</v>
+      </c>
+      <c r="AD127">
+        <v>4.1486000000000001</v>
+      </c>
+      <c r="AE127">
+        <v>4.2732999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="22:33" x14ac:dyDescent="0.25">
+      <c r="W128" t="s">
+        <v>13</v>
+      </c>
+      <c r="X128">
+        <v>0.44080000000000003</v>
+      </c>
+      <c r="Y128">
+        <v>0.34539999999999998</v>
+      </c>
+      <c r="Z128">
+        <v>0.28129999999999999</v>
+      </c>
+      <c r="AA128">
+        <v>0.18260000000000001</v>
+      </c>
+      <c r="AB128">
+        <v>0.2026</v>
+      </c>
+      <c r="AC128">
+        <v>0.23250000000000001</v>
+      </c>
+      <c r="AD128">
+        <v>0.26840000000000003</v>
+      </c>
+      <c r="AE128">
+        <v>0.31109999999999999</v>
+      </c>
+    </row>
+    <row r="129" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W129" t="s">
+        <v>14</v>
+      </c>
+      <c r="X129">
+        <v>7.3300000000000004E-2</v>
+      </c>
+      <c r="Y129">
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="Z129">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="AA129">
+        <v>0</v>
+      </c>
+      <c r="AB129">
+        <v>0</v>
+      </c>
+      <c r="AC129">
+        <v>0</v>
+      </c>
+      <c r="AD129">
+        <v>0</v>
+      </c>
+      <c r="AE129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="W130" t="s">
+        <v>18</v>
+      </c>
+      <c r="X130">
+        <v>0</v>
+      </c>
+      <c r="Y130">
+        <v>0</v>
+      </c>
+      <c r="Z130">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="AA130">
+        <v>20.510999999999999</v>
+      </c>
+      <c r="AB130">
+        <v>33.819299999999998</v>
+      </c>
+      <c r="AC130">
+        <v>51.9163</v>
+      </c>
+      <c r="AD130">
+        <v>60.128700000000002</v>
+      </c>
+      <c r="AE130">
+        <v>69.895899999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="X131">
+        <v>105.9659</v>
+      </c>
+      <c r="Y131">
+        <v>98.619399999999999</v>
+      </c>
+      <c r="Z131">
+        <v>114.10899999999999</v>
+      </c>
+      <c r="AA131">
+        <v>131.82839999999999</v>
+      </c>
+      <c r="AB131">
+        <v>147.7099</v>
+      </c>
+      <c r="AC131">
+        <v>169.75069999999999</v>
+      </c>
+      <c r="AD131">
+        <v>189.20880000000002</v>
+      </c>
+      <c r="AE131">
+        <v>212.33340000000004</v>
+      </c>
+    </row>
+    <row r="133" spans="23:31" x14ac:dyDescent="0.25">
+      <c r="X133">
+        <v>105.9659</v>
+      </c>
+      <c r="Y133">
+        <v>98.619399999999999</v>
+      </c>
+      <c r="Z133">
+        <v>114.10899999999999</v>
+      </c>
+      <c r="AA133">
+        <v>131.82839999999999</v>
+      </c>
+      <c r="AB133">
+        <v>147.7099</v>
+      </c>
+      <c r="AC133">
+        <v>169.75069999999999</v>
+      </c>
+      <c r="AD133">
+        <v>189.20880000000002</v>
+      </c>
+      <c r="AE133">
+        <v>212.33340000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>